<commit_message>
Add た form conversion game
</commit_message>
<xml_diff>
--- a/verbs.xlsx
+++ b/verbs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>benkyōshimasu</t>
+          <t>benkyoushimasu</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1198,17 +1198,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>のどが かわきます</t>
+          <t>のどがかわきます</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>のどが かわきます</t>
+          <t>のどがかわきます</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>nodoga kawakimasu</t>
+          <t>nodogakawakimasu</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1218,17 +1218,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>おなかが すきます</t>
+          <t>おなかがすきます</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>おなかが すきます</t>
+          <t>おなかがすきます</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>onakaga sukimasu</t>
+          <t>onakagasukimasu</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -1598,7 +1598,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>作ります、造ります</t>
+          <t>作ります</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1618,17 +1618,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>売ります</t>
+          <t>造ります</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>うります</t>
+          <t>つくります</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>urimasu</t>
+          <t>tsukurimasu</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -1638,17 +1638,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>知ります</t>
+          <t>売ります</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>しります</t>
+          <t>うります</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>shirimasu</t>
+          <t>urimasu</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1658,17 +1658,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>住みます</t>
+          <t>知ります</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>すみます</t>
+          <t>しります</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>sumimasu</t>
+          <t>shirimasu</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -1678,37 +1678,37 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>研究します</t>
+          <t>住みます</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>けんきゅうします</t>
+          <t>すみます</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>kenkyūshimasu</t>
+          <t>sumimasu</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>思い出します</t>
+          <t>研究します</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>おもいだします</t>
+          <t>けんきゅうします</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>omoidashimasu</t>
+          <t>kenkyuushimasu</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -1718,57 +1718,57 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>いらっしゃいます</t>
+          <t>思い出します</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>いらっしゃいます</t>
+          <t>おもいだします</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>irasshaimasu</t>
+          <t>omoidashimasu</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>乗り換えます</t>
+          <t>いらっしゃいます</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>のりかえます</t>
+          <t>いらっしゃいます</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>norikaemasu</t>
+          <t>irasshaimasu</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>入れます</t>
+          <t>乗り換えます</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>いれます</t>
+          <t>のりかえます</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>iremasu</t>
+          <t>norikaemasu</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -1778,37 +1778,37 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>出します</t>
+          <t>入れます</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>だします</t>
+          <t>いれます</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>dashimasu</t>
+          <t>iremasu</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>押します</t>
+          <t>出します</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>おします</t>
+          <t>だします</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>oshimasu</t>
+          <t>dashimasu</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -1818,17 +1818,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>飲みます</t>
+          <t>押します</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>のみます</t>
+          <t>おします</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>nomimasu</t>
+          <t>oshimasu</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -1838,57 +1838,57 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>始めます</t>
+          <t>飲みます</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>はじめます</t>
+          <t>のみます</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>hajimemasu</t>
+          <t>nomimasu</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>見学します</t>
+          <t>始めます</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>けんがくします</t>
+          <t>はじめます</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>kengakushimasu</t>
+          <t>hajimemasu</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>電話します</t>
+          <t>見学します</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>でんわします</t>
+          <t>けんがくします</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>denwashimasu</t>
+          <t>kengakushimasu</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -1898,37 +1898,37 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>覚えます</t>
+          <t>電話します</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>おぼえます</t>
+          <t>でんわします</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>oboemasu</t>
+          <t>denwashimasu</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>忘れます</t>
+          <t>覚えます</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>わすれます</t>
+          <t>おぼえます</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>wasuremasu</t>
+          <t>oboemasu</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -1938,57 +1938,57 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>なくします</t>
+          <t>忘れます</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>なくします</t>
+          <t>わすれます</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>nakushimasu</t>
+          <t>wasuremasu</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>払います</t>
+          <t>なくします</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>はらいます</t>
+          <t>なくします</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>haraimasu</t>
+          <t>nakushimasu</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>返します</t>
+          <t>払います</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>かえします</t>
+          <t>はらいます</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>kaeshimasu</t>
+          <t>haraimasu</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -1998,57 +1998,57 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>出かけます</t>
+          <t>返します</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>でかけます</t>
+          <t>かえします</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>dekakemasu</t>
+          <t>kaeshimasu</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>脱ぎます</t>
+          <t>出かけます</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ぬぎます</t>
+          <t>でかけます</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>nugimasu</t>
+          <t>dekakemasu</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>持って 行きます</t>
+          <t>脱ぎます</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>もって いきます</t>
+          <t>ぬぎます</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>motte ikimasu</t>
+          <t>nugimasu</t>
         </is>
       </c>
       <c r="D81" t="n">
@@ -2058,37 +2058,37 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>持って 来ます</t>
+          <t>持って行きます</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>もって きます</t>
+          <t>もっていきます</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>motte kimasu</t>
+          <t>motteikimasu</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>心配します</t>
+          <t>持って来ます</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>しんぱいします</t>
+          <t>もってきます</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>shinpaishimasu</t>
+          <t>mottekimasu</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -2098,17 +2098,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>残業します</t>
+          <t>心配します</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ざんぎょうします</t>
+          <t>しんぱいします</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>zangyōshimasu</t>
+          <t>shinpaishimasu</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -2118,17 +2118,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>出張します</t>
+          <t>残業します</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>しゅっちょうします</t>
+          <t>ざんぎょうします</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>shutchōshimasu</t>
+          <t>zangyoushimasu</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -2138,57 +2138,57 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>できます</t>
+          <t>出張します</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>できます</t>
+          <t>しゅっちょうします</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>dekimasu</t>
+          <t>shutchoushimasu</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>洗います</t>
+          <t>できます</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>あらいます</t>
+          <t>できます</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>araimasu</t>
+          <t>dekimasu</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>弾きます</t>
+          <t>洗います</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ひきます</t>
+          <t>あらいます</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>hikimasu</t>
+          <t>araimasu</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -2198,17 +2198,17 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>歌います</t>
+          <t>弾きます</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>うたいます</t>
+          <t>ひきます</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>utaimasu</t>
+          <t>hikimasu</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2218,37 +2218,37 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>集めます</t>
+          <t>歌います</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>あつめます</t>
+          <t>うたいます</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>atsumemasu</t>
+          <t>utaimasu</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>捨てます</t>
+          <t>集めます</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>すてます</t>
+          <t>あつめます</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>sutemasu</t>
+          <t>atsumemasu</t>
         </is>
       </c>
       <c r="D91" t="n">
@@ -2258,17 +2258,17 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>換えます</t>
+          <t>捨てます</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>かえます</t>
+          <t>すてます</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>kaemasu</t>
+          <t>sutemasu</t>
         </is>
       </c>
       <c r="D92" t="n">
@@ -2278,37 +2278,37 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>運転します</t>
+          <t>換えます</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>うんてんします</t>
+          <t>かえます</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>untenshimasu</t>
+          <t>kaemasu</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>予約します</t>
+          <t>運転します</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>よやくします</t>
+          <t>うんてんします</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>yoyakushimasu</t>
+          <t>untenshimasu</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -2318,177 +2318,177 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>登ります、上ります</t>
+          <t>予約します</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>のぼります</t>
+          <t>よやくします</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>noborimasu</t>
+          <t>yoyakushimasu</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>掃除します</t>
+          <t>登ります</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>そうじします</t>
+          <t>のぼります</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>sōjishimasu</t>
+          <t>noborimasu</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>洗濯します</t>
+          <t>上ります</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>せんたくします</t>
+          <t>のぼります</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>sentakushimasu</t>
+          <t>noborimasu</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>なります</t>
+          <t>掃除します</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>なります</t>
+          <t>そうじします</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>narimasu</t>
+          <t>soujishimasu</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>調べます</t>
+          <t>洗濯します</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>しらべます</t>
+          <t>せんたくします</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>shirabemasu</t>
+          <t>sentakushimasu</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>修理します</t>
+          <t>なります</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>しゅうりします</t>
+          <t>なります</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>shūrishimasu</t>
+          <t>narimasu</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>思います</t>
+          <t>調べます</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>おもいます</t>
+          <t>しらべます</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>omoimasu</t>
+          <t>shirabemasu</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>言います</t>
+          <t>修理します</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>いいます</t>
+          <t>しゅうりします</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>iimasu</t>
+          <t>shuurishimasu</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>勝ちます</t>
+          <t>思います</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>かちます</t>
+          <t>おもいます</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>kachimasu</t>
+          <t>omoimasu</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -2498,37 +2498,37 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>負けます</t>
+          <t>言います</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>まけます</t>
+          <t>いいます</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>makemasu</t>
+          <t>iimasu</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>動きます</t>
+          <t>勝ちます</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>うごきます</t>
+          <t>かちます</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>ugokimasu</t>
+          <t>kachimasu</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -2538,57 +2538,57 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>留学します</t>
+          <t>負けます</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>りゅうがくします</t>
+          <t>まけます</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>ryūgakushimasu</t>
+          <t>makemasu</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>着ます</t>
+          <t>役に立ちます</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>きます</t>
+          <t>やくにたちます</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>kimasu</t>
+          <t>yakunitachimasu</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>はきます</t>
+          <t>動きます</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>はきます</t>
+          <t>うごきます</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>hakimasu</t>
+          <t>ugokimasu</t>
         </is>
       </c>
       <c r="D108" t="n">
@@ -2598,37 +2598,37 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>かぶります</t>
+          <t>留学します</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>かぶります</t>
+          <t>りゅうがくします</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>kaburimasu</t>
+          <t>ryuugakushimasu</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>生まれます</t>
+          <t>着ます</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>うまれます</t>
+          <t>きます</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>umaremasu</t>
+          <t>kimasu</t>
         </is>
       </c>
       <c r="D110" t="n">
@@ -2638,17 +2638,17 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>回します</t>
+          <t>はきます</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>まわします</t>
+          <t>はきます</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>mawashimasu</t>
+          <t>hakimasu</t>
         </is>
       </c>
       <c r="D111" t="n">
@@ -2658,17 +2658,17 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>引きます</t>
+          <t>かぶります</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>ひきます</t>
+          <t>かぶります</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>hikimasu</t>
+          <t>kaburimasu</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -2678,17 +2678,17 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>変えます</t>
+          <t>生まれます</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>かえます</t>
+          <t>うまれます</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>kaemasu</t>
+          <t>umaremasu</t>
         </is>
       </c>
       <c r="D113" t="n">
@@ -2698,17 +2698,17 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>歩きます</t>
+          <t>回します</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>あるきます</t>
+          <t>まわします</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>arukimasu</t>
+          <t>mawashimasu</t>
         </is>
       </c>
       <c r="D114" t="n">
@@ -2718,37 +2718,37 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>引っ越しします</t>
+          <t>引きます</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>ひっこしします</t>
+          <t>ひきます</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>hikkoshishimasu</t>
+          <t>hikimasu</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>くれます</t>
+          <t>変えます</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>くれます</t>
+          <t>かえます</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>kuremasu</t>
+          <t>kaemasu</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -2758,17 +2758,17 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>直します</t>
+          <t>歩きます</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>なおします</t>
+          <t>あるきます</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>naoshimasu</t>
+          <t>arukimasu</t>
         </is>
       </c>
       <c r="D117" t="n">
@@ -2778,97 +2778,97 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>連れて 行きます</t>
+          <t>引っ越しします</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>つれて いきます</t>
+          <t>ひっこしします</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>tsurete ikimasu</t>
+          <t>hikkoshishimasu</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>連れて 来ます</t>
+          <t>くれます</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>つれて きます</t>
+          <t>くれます</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>tsurete kimasu</t>
+          <t>kuremasu</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>紹介します</t>
+          <t>直します</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>しょうかいします</t>
+          <t>なおします</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>shōkaishimasu</t>
+          <t>naoshimasu</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>案内します</t>
+          <t>連れて行きます</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>あんないします</t>
+          <t>つれていきます</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>annaishimasu</t>
+          <t>tsureteikimasu</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>説明します</t>
+          <t>連れて来ます</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>せつめいします</t>
+          <t>つれてきます</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>setsumeishimasu</t>
+          <t>tsuretekimasu</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -2878,77 +2878,77 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>飛びます</t>
+          <t>紹介します</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>とびます</t>
+          <t>しょうかいします</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>tobimasu</t>
+          <t>shoukaishimasu</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>登ります</t>
+          <t>案内します</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>のぼります</t>
+          <t>あんないします</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>noborimasu</t>
+          <t>annaishimasu</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>走ります</t>
+          <t>説明します</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>はしります</t>
+          <t>せつめいします</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>hashirimasu</t>
+          <t>setsumeishimasu</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>もぐります</t>
+          <t>飛びます</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>もぐります</t>
+          <t>とびます</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>mogurimasu</t>
+          <t>tobimasu</t>
         </is>
       </c>
       <c r="D126" t="n">
@@ -2958,17 +2958,17 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>飛び込みます</t>
+          <t>登ります</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>とびこみます</t>
+          <t>のぼります</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>tobikomimasu</t>
+          <t>noborimasu</t>
         </is>
       </c>
       <c r="D127" t="n">
@@ -2978,17 +2978,17 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>逆立ちます</t>
+          <t>走ります</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>さかだちます</t>
+          <t>はしります</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>sakadachimasu</t>
+          <t>hashirimasu</t>
         </is>
       </c>
       <c r="D128" t="n">
@@ -2998,17 +2998,17 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>ほいます</t>
+          <t>もぐります</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>ほいます</t>
+          <t>もぐります</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>hoimasu</t>
+          <t>mogurimasu</t>
         </is>
       </c>
       <c r="D129" t="n">
@@ -3018,17 +3018,17 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>けります</t>
+          <t>飛び込みます</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>けります</t>
+          <t>とびこみます</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>kerimasu</t>
+          <t>tobikomimasu</t>
         </is>
       </c>
       <c r="D130" t="n">
@@ -3038,17 +3038,17 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>振ります</t>
+          <t>逆立ちます</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>ふります</t>
+          <t>さかだちます</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>furimasu</t>
+          <t>sakadachimasu</t>
         </is>
       </c>
       <c r="D131" t="n">
@@ -3058,57 +3058,57 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>持ち上げます</t>
+          <t>ほいます</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>もちあげます</t>
+          <t>ほいます</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>mochiagemasu</t>
+          <t>hoimasu</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>投げます</t>
+          <t>けります</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>なげます</t>
+          <t>けります</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>nagemasu</t>
+          <t>kerimasu</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>たたきます</t>
+          <t>振ります</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>たたきます</t>
+          <t>ふります</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>tatakimasu</t>
+          <t>furimasu</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -3118,77 +3118,77 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>引きます</t>
+          <t>持ち上げます</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>ひきます</t>
+          <t>もちあげます</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>hikimasu</t>
+          <t>mochiagemasu</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>押します</t>
+          <t>投げます</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>おします</t>
+          <t>なげます</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>oshimasu</t>
+          <t>nagemasu</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>曲げます</t>
+          <t>たたきます</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>まげます</t>
+          <t>たたきます</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>magemasu</t>
+          <t>tatakimasu</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>伸ばします</t>
+          <t>引きます</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>のばします</t>
+          <t>ひきます</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>nobashimasu</t>
+          <t>hikimasu</t>
         </is>
       </c>
       <c r="D138" t="n">
@@ -3198,17 +3198,17 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>転びます</t>
+          <t>押します</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>ころびます</t>
+          <t>おします</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>korobimasu</t>
+          <t>oshimasu</t>
         </is>
       </c>
       <c r="D139" t="n">
@@ -3218,20 +3218,80 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
+          <t>曲げます</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>まげます</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>magemasu</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>伸ばします</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>のばします</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>nobashimasu</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>転びます</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>ころびます</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>korobimasu</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
           <t>振り向きますます</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
+      <c r="B143" t="inlineStr">
         <is>
           <t>ふりむきます</t>
         </is>
       </c>
-      <c r="C140" t="inlineStr">
+      <c r="C143" t="inlineStr">
         <is>
           <t>furimukimasu</t>
         </is>
       </c>
-      <c r="D140" t="n">
+      <c r="D143" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>